<commit_message>
final version for advanced system lab
</commit_message>
<xml_diff>
--- a/measurements/avx_optimizations/avx_performance.xlsx
+++ b/measurements/avx_optimizations/avx_performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kehongliu/Downloads/team38/measurements/avx_optimizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134A739A-6BBB-1E4D-BFDC-2EBD9F8B11E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62087206-4437-7847-A357-3D8BCEBB291D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" activeTab="3" xr2:uid="{73580FC9-1AEE-E945-B371-EE598F750A28}"/>
   </bookViews>
@@ -855,7 +855,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -900,7 +900,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1785,237 +1785,276 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="baseline"/>
-      <sheetName val="opt3"/>
-      <sheetName val="opt4"/>
-      <sheetName val="baseline plot"/>
-      <sheetName val="comparison_plot"/>
+      <sheetName val="plotting_report"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="0">
         <row r="1">
           <cell r="B1" t="str">
-            <v>baseline</v>
+            <v>Baseline</v>
           </cell>
           <cell r="C1" t="str">
-            <v>optimized_3</v>
+            <v>Optimization 3</v>
           </cell>
           <cell r="D1" t="str">
-            <v>optimized_4</v>
+            <v>Optimization 5</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Optimization 2</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>Optimization 1</v>
           </cell>
         </row>
         <row r="2">
           <cell r="A2" t="str">
-            <v>2^0</v>
+            <v>2^3</v>
           </cell>
           <cell r="B2">
-            <v>1.5725141526273738</v>
+            <v>0.86560955997421385</v>
           </cell>
           <cell r="C2">
-            <v>1.7300663912977658</v>
+            <v>0.62584386420884708</v>
           </cell>
           <cell r="D2">
-            <v>1.6531339286452293</v>
+            <v>1.1059708266882087</v>
+          </cell>
+          <cell r="E2">
+            <v>0.85749552600000001</v>
+          </cell>
+          <cell r="F2">
+            <v>1.7610317760961298</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>2^1</v>
+            <v>2^4</v>
           </cell>
           <cell r="B3">
-            <v>1.1034949648811034</v>
+            <v>0.81843076693438654</v>
           </cell>
           <cell r="C3">
-            <v>1.29235855436171</v>
+            <v>1.0111894775974826</v>
           </cell>
           <cell r="D3">
-            <v>2.5833777664296069</v>
+            <v>1.1375738669029152</v>
+          </cell>
+          <cell r="E3">
+            <v>0.81377294700000002</v>
+          </cell>
+          <cell r="F3">
+            <v>1.2566574417029674</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4" t="str">
-            <v>2^2</v>
+            <v>2^5</v>
           </cell>
           <cell r="B4">
-            <v>0.95738386790254049</v>
+            <v>0.7697677405663802</v>
           </cell>
           <cell r="C4">
-            <v>1.1102425315904569</v>
+            <v>1.0611232668445225</v>
           </cell>
           <cell r="D4">
-            <v>4.4149762921282001</v>
+            <v>1.1417055922177923</v>
+          </cell>
+          <cell r="E4">
+            <v>0.762879894</v>
+          </cell>
+          <cell r="F4">
+            <v>1.0735796931997152</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>2^3</v>
+            <v>2^6</v>
           </cell>
           <cell r="B5">
-            <v>0.86560955997421385</v>
+            <v>0.63439960197840151</v>
           </cell>
           <cell r="C5">
-            <v>0.95750846621417729</v>
+            <v>1.0820083808601728</v>
           </cell>
           <cell r="D5">
-            <v>1.7610317760961298</v>
+            <v>1.1378481999395473</v>
+          </cell>
+          <cell r="E5">
+            <v>0.67276005800000005</v>
+          </cell>
+          <cell r="F5">
+            <v>0.97161035821085451</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6" t="str">
-            <v>2^4</v>
+            <v>2^7</v>
           </cell>
           <cell r="B6">
-            <v>0.81843076693438654</v>
+            <v>0.51546663788036895</v>
           </cell>
           <cell r="C6">
-            <v>0.92871222279206855</v>
+            <v>1.0968486407310563</v>
           </cell>
           <cell r="D6">
-            <v>1.2566574417029674</v>
+            <v>1.1427183621096177</v>
+          </cell>
+          <cell r="E6">
+            <v>0.55452903200000003</v>
+          </cell>
+          <cell r="F6">
+            <v>0.8572433962264151</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7" t="str">
-            <v>2^5</v>
+            <v>2^8</v>
           </cell>
           <cell r="B7">
-            <v>0.7697677405663802</v>
+            <v>0.48548168403614972</v>
           </cell>
           <cell r="C7">
-            <v>0.88461848225642004</v>
+            <v>1.1020135876640123</v>
           </cell>
           <cell r="D7">
-            <v>1.0735796931997152</v>
+            <v>1.1375827831360736</v>
+          </cell>
+          <cell r="E7">
+            <v>0.503378824</v>
+          </cell>
+          <cell r="F7">
+            <v>0.7750728051391863</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8" t="str">
-            <v>2^6</v>
+            <v>2^9</v>
           </cell>
           <cell r="B8">
-            <v>0.63439960197840151</v>
+            <v>0.4654133181621522</v>
           </cell>
           <cell r="C8">
-            <v>0.75357522362624885</v>
+            <v>1.104190141062444</v>
           </cell>
           <cell r="D8">
-            <v>0.97161035821085451</v>
+            <v>1.1392499363057325</v>
+          </cell>
+          <cell r="E8">
+            <v>0.474364444</v>
+          </cell>
+          <cell r="F8">
+            <v>0.74474917525773199</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9" t="str">
-            <v>2^7</v>
+            <v>2^10</v>
           </cell>
           <cell r="B9">
-            <v>0.51546663788036895</v>
+            <v>0.45970564753836046</v>
           </cell>
           <cell r="C9">
-            <v>0.61397162162162167</v>
+            <v>1.1138803963706572</v>
           </cell>
           <cell r="D9">
-            <v>0.8572433962264151</v>
+            <v>1.1373250955414014</v>
+          </cell>
+          <cell r="E9">
+            <v>0.46655015399999999</v>
+          </cell>
+          <cell r="F9">
+            <v>0.73544078980891725</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>2^8</v>
+            <v>2^11</v>
           </cell>
           <cell r="B10">
-            <v>0.48548168403614972</v>
+            <v>0.45663243356350702</v>
           </cell>
           <cell r="C10">
-            <v>0.56467862714508577</v>
+            <v>1.1077346289368704</v>
           </cell>
           <cell r="D10">
-            <v>0.7750728051391863</v>
+            <v>1.1418174080000001</v>
+          </cell>
+          <cell r="E10">
+            <v>0.46038953599999999</v>
+          </cell>
+          <cell r="F10">
+            <v>0.72809955205047316</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11" t="str">
-            <v>2^9</v>
+            <v>2^12</v>
           </cell>
           <cell r="B11">
-            <v>0.4654133181621522</v>
+            <v>0.45805154239823637</v>
           </cell>
           <cell r="C11">
-            <v>0.53314147601476014</v>
+            <v>1.1125739942486719</v>
           </cell>
           <cell r="D11">
-            <v>0.74474917525773199</v>
+            <v>1.1390559201596806</v>
+          </cell>
+          <cell r="E11">
+            <v>0.46172322500000001</v>
+          </cell>
+          <cell r="F11">
+            <v>0.73253059523809527</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12" t="str">
-            <v>2^10</v>
+            <v>2^13</v>
           </cell>
           <cell r="B12">
-            <v>0.45970564753836046</v>
+            <v>0.45941750584778773</v>
           </cell>
           <cell r="C12">
-            <v>0.51546519642857147</v>
+            <v>1.1147290147999804</v>
           </cell>
           <cell r="D12">
-            <v>0.73544078980891725</v>
+            <v>1.1410923559999999</v>
+          </cell>
+          <cell r="E12">
+            <v>0.45802418099999997</v>
+          </cell>
+          <cell r="F12">
+            <v>0.70717832452107277</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13" t="str">
-            <v>2^11</v>
+            <v>2^14</v>
           </cell>
           <cell r="B13">
-            <v>0.45663243356350702</v>
+            <v>0.46038349986973026</v>
           </cell>
           <cell r="C13">
-            <v>0.52218904524886878</v>
+            <v>1.1115190451023991</v>
           </cell>
           <cell r="D13">
-            <v>0.72809955205047316</v>
+            <v>1.140971521</v>
+          </cell>
+          <cell r="E13">
+            <v>0.46071321300000001</v>
+          </cell>
+          <cell r="F13">
+            <v>0.72023984107317074</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14" t="str">
-            <v>2^12</v>
-          </cell>
-          <cell r="B14">
-            <v>0.45805154239823637</v>
+            <v>2^15</v>
           </cell>
           <cell r="C14">
-            <v>0.52742202857142861</v>
+            <v>1.1131247282217642</v>
           </cell>
           <cell r="D14">
-            <v>0.73253059523809527</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>2^13</v>
-          </cell>
-          <cell r="B15">
-            <v>0.45941750584778773</v>
-          </cell>
-          <cell r="C15">
-            <v>0.52962279110473454</v>
-          </cell>
-          <cell r="D15">
-            <v>0.70717832452107277</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>2^14</v>
-          </cell>
-          <cell r="B16">
-            <v>0.46038349986973026</v>
-          </cell>
-          <cell r="C16">
-            <v>0.52920848537634413</v>
-          </cell>
-          <cell r="D16">
-            <v>0.72023984107317074</v>
+            <v>1.14091110425</v>
           </cell>
         </row>
       </sheetData>
@@ -2655,7 +2694,7 @@
         <v>1094.19</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C3:C17" si="1">A4*(59+34*A4)+8</f>
+        <f t="shared" ref="C4:C17" si="1">A4*(59+34*A4)+8</f>
         <v>788</v>
       </c>
       <c r="D4">
@@ -3143,8 +3182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BDC0B7-37F8-C740-921F-98500B21EC14}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="81" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>